<commit_message>
Added feature to update box information
</commit_message>
<xml_diff>
--- a/PEL - FECHAMENTO ESTOQUE.xlsx
+++ b/PEL - FECHAMENTO ESTOQUE.xlsx
@@ -1334,7 +1334,7 @@
       <c r="B59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="10">
         <v>100</v>
       </c>
       <c r="D59" s="3"/>
@@ -1346,7 +1346,7 @@
       <c r="B60" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="10">
         <v>101</v>
       </c>
       <c r="D60" s="3"/>

</xml_diff>